<commit_message>
archiving additional steady state model runs including current best run 17_20211208
</commit_message>
<xml_diff>
--- a/MODFLOW/modflow_calibration/ss_calibration/manual_calib_results/tables/manual_calib_results_20211203.xlsx
+++ b/MODFLOW/modflow_calibration/ss_calibration/manual_calib_results/tables/manual_calib_results_20211203.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\projects\russian_river\model\RR_GSFLOW\MODFLOW\modflow_calibration\ss_calibration\manual_calib_results\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E31FDDD-2375-4490-B573-5FBA4A1770D5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C0E5A7-C9D7-4308-BAA3-BE56B57DB490}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EE8E39C0-44A7-43F0-83A8-ECA6A11E6594}"/>
+    <workbookView xWindow="16395" yWindow="2355" windowWidth="17610" windowHeight="17175" xr2:uid="{EE8E39C0-44A7-43F0-83A8-ECA6A11E6594}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -175,10 +175,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -494,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4747756-D7B7-4DCB-BF6C-AF4FEF512672}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="196" zoomScaleNormal="196" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" zoomScale="196" zoomScaleNormal="196" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,7 +615,7 @@
       <c r="C10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -626,19 +626,19 @@
       <c r="C11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="3"/>
+      <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -649,13 +649,13 @@
       <c r="C13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="3"/>
+      <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -693,6 +693,11 @@
       </c>
       <c r="D17" s="1" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>20211207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated steady state model results plotting code
</commit_message>
<xml_diff>
--- a/MODFLOW/modflow_calibration/ss_calibration/manual_calib_results/tables/manual_calib_results_20211203.xlsx
+++ b/MODFLOW/modflow_calibration/ss_calibration/manual_calib_results/tables/manual_calib_results_20211203.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\projects\russian_river\model\RR_GSFLOW\MODFLOW\modflow_calibration\ss_calibration\manual_calib_results\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C0E5A7-C9D7-4308-BAA3-BE56B57DB490}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA28ECA5-6C40-4165-B2ED-62EE82775FF1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16395" yWindow="2355" windowWidth="17610" windowHeight="17175" xr2:uid="{EE8E39C0-44A7-43F0-83A8-ECA6A11E6594}"/>
+    <workbookView xWindow="14190" yWindow="750" windowWidth="20760" windowHeight="17910" xr2:uid="{EE8E39C0-44A7-43F0-83A8-ECA6A11E6594}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
   <si>
     <t>id</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>20211203_10</t>
+  </si>
+  <si>
+    <t>20211210_01</t>
   </si>
 </sst>
 </file>
@@ -494,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4747756-D7B7-4DCB-BF6C-AF4FEF512672}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="196" zoomScaleNormal="196" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,6 +703,11 @@
         <v>20211207</v>
       </c>
     </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="D10:D11"/>

</xml_diff>